<commit_message>
(update) 动画Table + 剑Table.简化SO
</commit_message>
<xml_diff>
--- a/Excels/Weapon.xlsx
+++ b/Excels/Weapon.xlsx
@@ -7,14 +7,14 @@
     <workbookView windowWidth="27195" windowHeight="13140"/>
   </bookViews>
   <sheets>
-    <sheet name="WeaponTest1" sheetId="1" r:id="rId1"/>
+    <sheet name="SwordMeta" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>ID</t>
   </si>
@@ -25,6 +25,15 @@
     <t>攻击次数</t>
   </si>
   <si>
+    <t>最大间隔</t>
+  </si>
+  <si>
+    <t>描述</t>
+  </si>
+  <si>
+    <t>动画索引</t>
+  </si>
+  <si>
     <t>id</t>
   </si>
   <si>
@@ -34,13 +43,43 @@
     <t>numOfAttack</t>
   </si>
   <si>
+    <t>maxInterval</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>animIDs</t>
+  </si>
+  <si>
     <t>int</t>
   </si>
   <si>
     <t>string</t>
   </si>
   <si>
-    <t>233之剑</t>
+    <t>float</t>
+  </si>
+  <si>
+    <t>int[]</t>
+  </si>
+  <si>
+    <t>绿色的剑</t>
+  </si>
+  <si>
+    <t>绿色的一把剑</t>
+  </si>
+  <si>
+    <t>0,1,2</t>
+  </si>
+  <si>
+    <t>红色的剑</t>
+  </si>
+  <si>
+    <t>红色的一把剑</t>
+  </si>
+  <si>
+    <t>3,4,5</t>
   </si>
 </sst>
 </file>
@@ -975,19 +1014,23 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="3" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="13.375" customWidth="1"/>
-    <col min="3" max="3" width="20.375" customWidth="1"/>
+    <col min="1" max="1" width="20.375" customWidth="1"/>
+    <col min="2" max="2" width="20.125" customWidth="1"/>
+    <col min="3" max="3" width="24.375" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="18.625" customWidth="1"/>
+    <col min="6" max="6" width="26.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -997,38 +1040,94 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>3</v>
+      </c>
+      <c r="D4">
+        <v>1.5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1.5</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>